<commit_message>
Atualização das extrações de links para todos os cursos
</commit_message>
<xml_diff>
--- a/data/licenciaturas_links_full.xlsx
+++ b/data/licenciaturas_links_full.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C74"/>
+  <dimension ref="A1:C167"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,12 +458,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Cecília Calado</t>
+          <t>António Silvestre</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docentes/cecilia-ribeiro-da-cruz-calado</t>
+          <t>https://www.isel.pt/docentes/antonio-jorge-duarte-de-castro-silvestre</t>
         </is>
       </c>
     </row>
@@ -475,12 +475,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Descarregar</t>
+          <t>Apresentação</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>https://isel.pt/sites/default/files/001_imagens_isel/pdf/flyers_2025_04/FolhetoISEL-LEB.pdf</t>
+          <t>https://www.isel.pt/curso/licenciatura/licenciatura-em-engenharia-biomedica</t>
         </is>
       </c>
     </row>
@@ -492,12 +492,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>João Ramos da Costa</t>
+          <t>Cecília Calado</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docente/joao-pedro-barrigana-ramos-da-costa-estesl</t>
+          <t>https://www.isel.pt/docentes/cecilia-ribeiro-da-cruz-calado</t>
         </is>
       </c>
     </row>
@@ -509,12 +509,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Luís Minhalma</t>
+          <t>Congresso do 30.º Aniversário da PROFORUM</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docentes/luis-miguel-minhalma</t>
+          <t>https://www.isel.pt/eventos/congresso-do-30o-aniversario-da-proforum</t>
         </is>
       </c>
     </row>
@@ -526,886 +526,886 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Manuel Matos</t>
+          <t>Descarregar</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docentes/manuel-jose-de-matos</t>
+          <t>https://isel.pt/sites/default/files/001_imagens_isel/pdf/flyers_2025_04/FolhetoISEL-LEB.pdf</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Engenharia Civil</t>
+          <t>Engenharia Biomédica</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Descarregar</t>
+          <t>Fundação Santander e ISEL atribuem Incentivo à Investigação Exploratória</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>https://isel.pt/sites/default/files/001_imagens_isel/pdf/flyers_2025_04/FolhetoISEL-LEC.pdf</t>
+          <t>https://www.isel.pt/noticias/fundacao-santander-e-isel-atribuem-incentivo-investigacao-exploratoria</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Engenharia Civil</t>
+          <t>Engenharia Biomédica</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Idália Gomes</t>
+          <t>Horários</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docentes/maria-idalia-da-silva-gomes</t>
+          <t>https://www.isel.pt/comunidade/estudantes/informacoes-academicas/horarios</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Engenharia Civil</t>
+          <t>Engenharia Biomédica</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Jorge Reis de Barros</t>
+          <t>João Ramos da Costa</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docentes/jorge-alexandre-dias-dos-reis-de-barros</t>
+          <t>https://www.isel.pt/docente/joao-pedro-barrigana-ramos-da-costa-estesl</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Engenharia Civil</t>
+          <t>Engenharia Biomédica</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Luís Evangelista</t>
+          <t>Luís Minhalma</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docentes/luis-manuel-faria-da-rocha-evangelista</t>
+          <t>https://www.isel.pt/docentes/luis-miguel-minhalma</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Engenharia Civil</t>
+          <t>Engenharia Biomédica</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Maria do Carmo Conde</t>
+          <t>Manuel Matos</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docentes/maria-do-carmo-cachao-conde</t>
+          <t>https://www.isel.pt/docentes/manuel-jose-de-matos</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Engenharia Civil</t>
+          <t>Engenharia Biomédica</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Paulo Mendes</t>
+          <t>Mapa de testes e exames</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docentes/paulo-jorge-henriques-mendes</t>
+          <t>https://www.isel.pt/comunidade/estudantes/informacoes-academicas/testes_e_exames</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Engenharia Eletrotécnica</t>
+          <t>Engenharia Biomédica</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Ana Martins</t>
+          <t>Modalidades de ingresso</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docentes/ana-alexandra-antunes-figueiredo-martins</t>
+          <t>https://www.isel.pt/ensino/candidatos/modalidades-de-ingresso</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Engenharia Eletrotécnica</t>
+          <t>Engenharia Biomédica</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Descarregar</t>
+          <t>Plano de Estudos</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>https://isel.pt/sites/default/files/001_imagens_isel/pdf/flyers_2025_04/FolhetoISEL-LEE.pdf</t>
+          <t>https://www.isel.pt/curso/10538/plano-de-estudos</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Engenharia Eletrotécnica</t>
+          <t>Engenharia Biomédica</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>José Gabriel Lopes</t>
+          <t>Propinas</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docentes/jose-gabriel-da-silva-lopes</t>
+          <t>https://www.isel.pt/comunidade/estudantes/informacoes-academicas/propinas</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Engenharia Eletrotécnica</t>
+          <t>Engenharia Civil</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Luís Rocha da Encarnação</t>
+          <t>Apresentação</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docentes/luis-jose-lamy-rocha-da-encarnacao</t>
+          <t>https://www.isel.pt/curso/licenciatura/licenciatura-em-engenharia-civil</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Engenharia Eletrotécnica</t>
+          <t>Engenharia Civil</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Miguel Chaves</t>
+          <t>Congresso do 30.º Aniversário da PROFORUM</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docentes/miguel-cabral-ferreira-chaves</t>
+          <t>https://www.isel.pt/eventos/congresso-do-30o-aniversario-da-proforum</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Engenharia Eletrotécnica</t>
+          <t>Engenharia Civil</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Ricardo Luís</t>
+          <t>Descarregar</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docentes/ricardo-jorge-ferreira-luis</t>
+          <t>https://isel.pt/sites/default/files/001_imagens_isel/pdf/flyers_2025_04/FolhetoISEL-LEC.pdf</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Engenharia Eletrónica e Telecomunicações e de Computadores</t>
+          <t>Engenharia Civil</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>António Serrador</t>
+          <t>Fundação Santander e ISEL atribuem Incentivo à Investigação Exploratória</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docentes/antonio-joao-nunes-serrador</t>
+          <t>https://www.isel.pt/noticias/fundacao-santander-e-isel-atribuem-incentivo-investigacao-exploratoria</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Engenharia Eletrónica e Telecomunicações e de Computadores</t>
+          <t>Engenharia Civil</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Carlos Meneses</t>
+          <t>Horários</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docentes/carlos-eduardo-de-meneses-ribeiro</t>
+          <t>https://www.isel.pt/comunidade/estudantes/informacoes-academicas/horarios</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Engenharia Eletrónica e Telecomunicações e de Computadores</t>
+          <t>Engenharia Civil</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Descarregar</t>
+          <t>Idália Gomes</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>https://isel.pt/sites/default/files/001_imagens_isel/pdf/flyers_2025_04/FolhetoISEL-LEETC.pdf</t>
+          <t>https://www.isel.pt/docentes/maria-idalia-da-silva-gomes</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Engenharia Eletrónica e Telecomunicações e de Computadores</t>
+          <t>Engenharia Civil</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Jorge Martins Pião</t>
+          <t>Jorge Reis de Barros</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docentes/jorge-manuel-rodrigues-martins-piao</t>
+          <t>https://www.isel.pt/docentes/jorge-alexandre-dias-dos-reis-de-barros</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Engenharia Eletrónica e Telecomunicações e de Computadores</t>
+          <t>Engenharia Civil</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Pedro Sampaio</t>
+          <t>Luís Evangelista</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docentes/pedro-miguel-fernandes-sampaio</t>
+          <t>https://www.isel.pt/docentes/luis-manuel-faria-da-rocha-evangelista</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Engenharia Eletrónica e Telecomunicações e de Computadores</t>
+          <t>Engenharia Civil</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Vitor Costa</t>
+          <t>Mapa de testes e exames</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docentes/vitor-manuel-da-silva-costa</t>
+          <t>https://www.isel.pt/comunidade/estudantes/informacoes-academicas/testes_e_exames</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Engenharia Física Aplicada</t>
+          <t>Engenharia Civil</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Descarregar</t>
+          <t>Maria do Carmo Conde</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>https://isel.pt/sites/default/files/001_imagens_isel/pdf/flyers_2025_04/FolhetoISEL-LEFA.pdf</t>
+          <t>https://www.isel.pt/docentes/maria-do-carmo-cachao-conde</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Engenharia Física Aplicada</t>
+          <t>Engenharia Civil</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Pedro Ferreira</t>
+          <t>Modalidades de ingresso</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docentes/pedro-miguel-martins-ferreira</t>
+          <t>https://www.isel.pt/ensino/candidatos/modalidades-de-ingresso</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Engenharia Física Aplicada</t>
+          <t>Engenharia Civil</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Pedro Patrício</t>
+          <t>Paulo Mendes</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docentes/pedro-manuel-alves-patricio-da-silva</t>
+          <t>https://www.isel.pt/docentes/paulo-jorge-henriques-mendes</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Engenharia Física Aplicada</t>
+          <t>Engenharia Civil</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Vitor Oliveira</t>
+          <t>Plano de Estudos</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docentes/vitor-manuel-barbas-de-oliveira</t>
+          <t>https://www.isel.pt/curso/36831/plano-de-estudos</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Engenharia Informática e Multimédia</t>
+          <t>Engenharia Civil</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>António Teófilo</t>
+          <t>Propinas</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docentes/antonio-gelasio-frazao-isidro-teofilo</t>
+          <t>https://www.isel.pt/comunidade/estudantes/informacoes-academicas/propinas</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Engenharia Informática e Multimédia</t>
+          <t>Engenharia Eletrotécnica</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Descarregar</t>
+          <t>Ana Martins</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>https://isel.pt/sites/default/files/001_imagens_isel/pdf/flyers_2025_04/FolhetoISEL-LEIM.pdf</t>
+          <t>https://www.isel.pt/docentes/ana-alexandra-antunes-figueiredo-martins</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Engenharia Informática e Multimédia</t>
+          <t>Engenharia Eletrotécnica</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Filipa Almeida</t>
+          <t>Apresentação</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docentes/filipa-soares-de-almeida</t>
+          <t>https://www.isel.pt/curso/licenciatura/licenciatura-em-engenharia-eletrotecnica</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Engenharia Informática e Multimédia</t>
+          <t>Engenharia Eletrotécnica</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Gonçalo Valadão Matias</t>
+          <t>Congresso do 30.º Aniversário da PROFORUM</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docentes/goncalo-ramiro-valadao-matias</t>
+          <t>https://www.isel.pt/eventos/congresso-do-30o-aniversario-da-proforum</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Engenharia Informática e Multimédia</t>
+          <t>Engenharia Eletrotécnica</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Manfred Niehus</t>
+          <t>Descarregar</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docentes/manfred-niehus</t>
+          <t>https://isel.pt/sites/default/files/001_imagens_isel/pdf/flyers_2025_04/FolhetoISEL-LEE.pdf</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Engenharia Informática e Multimédia</t>
+          <t>Engenharia Eletrotécnica</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Rui Jesus</t>
+          <t>Fundação Santander e ISEL atribuem Incentivo à Investigação Exploratória</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docentes/rui-manuel-feliciano-de-jesus</t>
+          <t>https://www.isel.pt/noticias/fundacao-santander-e-isel-atribuem-incentivo-investigacao-exploratoria</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Engenharia Informática e de Computadores</t>
+          <t>Engenharia Eletrotécnica</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Artur Ferreira</t>
+          <t>Horários</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docentes/artur-jorge-ferreira</t>
+          <t>https://www.isel.pt/comunidade/estudantes/informacoes-academicas/horarios</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Engenharia Informática e de Computadores</t>
+          <t>Engenharia Eletrotécnica</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Cátia Vaz</t>
+          <t>José Gabriel Lopes</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docentes/catia-raquel-jesus-vaz</t>
+          <t>https://www.isel.pt/docentes/jose-gabriel-da-silva-lopes</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Engenharia Informática e de Computadores</t>
+          <t>Engenharia Eletrotécnica</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Descarregar</t>
+          <t>Luís Rocha da Encarnação</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>https://isel.pt/sites/default/files/001_imagens_isel/pdf/flyers_2025_04/FolhetoISEL-LEIC.pdf</t>
+          <t>https://www.isel.pt/docentes/luis-jose-lamy-rocha-da-encarnacao</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Engenharia Informática e de Computadores</t>
+          <t>Engenharia Eletrotécnica</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Nuno Leite</t>
+          <t>Mapa de testes e exames</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docentes/nuno-miguel-da-costa-de-sousa-leite</t>
+          <t>https://www.isel.pt/comunidade/estudantes/informacoes-academicas/testes_e_exames</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Engenharia Informática e de Computadores</t>
+          <t>Engenharia Eletrotécnica</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Pedro Miguens Matutino</t>
+          <t>Miguel Chaves</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docentes/pedro-miguel-florindo-miguens-matutino</t>
+          <t>https://www.isel.pt/docentes/miguel-cabral-ferreira-chaves</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Engenharia Informática, Redes e Telecomunicações</t>
+          <t>Engenharia Eletrotécnica</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Descarregar</t>
+          <t>Modalidades de ingresso</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>https://isel.pt/sites/default/files/001_imagens_isel/pdf/flyers_2025_04/FolhetoISEL-LEIRT.pdf</t>
+          <t>https://www.isel.pt/ensino/candidatos/modalidades-de-ingresso</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Engenharia Informática, Redes e Telecomunicações</t>
+          <t>Engenharia Eletrotécnica</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Filipe Freitas</t>
+          <t>Plano de Estudos</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docentes/filipe-bastos-de-freitas</t>
+          <t>https://www.isel.pt/curso/10515/plano-de-estudos</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Engenharia Informática, Redes e Telecomunicações</t>
+          <t>Engenharia Eletrotécnica</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Isabel Matos</t>
+          <t>Propinas</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docentes/isabel-maria-teixeira-de-matos</t>
+          <t>https://www.isel.pt/comunidade/estudantes/informacoes-academicas/propinas</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Engenharia Informática, Redes e Telecomunicações</t>
+          <t>Engenharia Eletrotécnica</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>João Trindade</t>
+          <t>Ricardo Luís</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docentes/joao-humberto-holbeche-trindade</t>
+          <t>https://www.isel.pt/docentes/ricardo-jorge-ferreira-luis</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Engenharia Informática, Redes e Telecomunicações</t>
+          <t>Engenharia Eletrónica e Telecomunicações e de Computadores</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Luis Mata</t>
+          <t>António Serrador</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docente/luis-miguel-maia-bravo-da-mata</t>
+          <t>https://www.isel.pt/docentes/antonio-joao-nunes-serrador</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Engenharia Informática, Redes e Telecomunicações</t>
+          <t>Engenharia Eletrónica e Telecomunicações e de Computadores</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Pedro Vieira</t>
+          <t>Apresentação</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docentes/pedro-manuel-de-almeida-carvalho-vieira</t>
+          <t>https://www.isel.pt/curso/licenciatura/licenciatura-em-engenharia-eletronica-e-telecomunicacoes-e-de-computadores</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Engenharia Mecânica</t>
+          <t>Engenharia Eletrónica e Telecomunicações e de Computadores</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Cláudia Casaca</t>
+          <t>Carlos Meneses</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docentes/claudia-sofia-seneca-da-luz-casaca</t>
+          <t>https://www.isel.pt/docentes/carlos-eduardo-de-meneses-ribeiro</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Engenharia Mecânica</t>
+          <t>Engenharia Eletrónica e Telecomunicações e de Computadores</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Descarregar</t>
+          <t>Congresso do 30.º Aniversário da PROFORUM</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>https://isel.pt/sites/default/files/001_imagens_isel/pdf/flyers_2025_04/FolhetoISEL-LEM.pdf</t>
+          <t>https://www.isel.pt/eventos/congresso-do-30o-aniversario-da-proforum</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Engenharia Mecânica</t>
+          <t>Engenharia Eletrónica e Telecomunicações e de Computadores</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Fernando Carreira</t>
+          <t>Descarregar</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docentes/fernando-paulo-neves-da-fonseca-carreira</t>
+          <t>https://isel.pt/sites/default/files/001_imagens_isel/pdf/flyers_2025_04/FolhetoISEL-LEETC.pdf</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Engenharia Mecânica</t>
+          <t>Engenharia Eletrónica e Telecomunicações e de Computadores</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>José Sobral</t>
+          <t>Fundação Santander e ISEL atribuem Incentivo à Investigação Exploratória</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docentes/jose-augusto-da-silva-sobral</t>
+          <t>https://www.isel.pt/noticias/fundacao-santander-e-isel-atribuem-incentivo-investigacao-exploratoria</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Engenharia Mecânica</t>
+          <t>Engenharia Eletrónica e Telecomunicações e de Computadores</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Ricardo Portal</t>
+          <t>Horários</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docentes/ricardo-jose-fontes-portal</t>
+          <t>https://www.isel.pt/comunidade/estudantes/informacoes-academicas/horarios</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Engenharia Mecânica</t>
+          <t>Engenharia Eletrónica e Telecomunicações e de Computadores</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Teresa Moura e Silva</t>
+          <t>Jorge Martins Pião</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docentes/maria-teresa-oliveira-moura-e-silva</t>
+          <t>https://www.isel.pt/docentes/jorge-manuel-rodrigues-martins-piao</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Engenharia Química e Biológica</t>
+          <t>Engenharia Eletrónica e Telecomunicações e de Computadores</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Alexandra Costa</t>
+          <t>Mapa de testes e exames</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docentes/alexandra-isabel-martins-paulo-costa</t>
+          <t>https://www.isel.pt/comunidade/estudantes/informacoes-academicas/testes_e_exames</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Engenharia Química e Biológica</t>
+          <t>Engenharia Eletrónica e Telecomunicações e de Computadores</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Ana Figueiredo</t>
+          <t>Modalidades de ingresso</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docentes/ana-sofia-de-oliveira-figueiredo</t>
+          <t>https://www.isel.pt/ensino/candidatos/modalidades-de-ingresso</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Engenharia Química e Biológica</t>
+          <t>Engenharia Eletrónica e Telecomunicações e de Computadores</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Descarregar</t>
+          <t>Pedro Sampaio</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>https://isel.pt/sites/default/files/001_imagens_isel/pdf/flyers_2025_04/FolhetoISEL-LEQB.pdf</t>
+          <t>https://www.isel.pt/docentes/pedro-miguel-fernandes-sampaio</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Engenharia Química e Biológica</t>
+          <t>Engenharia Eletrónica e Telecomunicações e de Computadores</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Magda Semedo</t>
+          <t>Plano de Estudos</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docentes/magda-sofia-soares-de-carvalho-cardoso-nobre-semedo</t>
+          <t>https://www.isel.pt/curso/10519/plano-de-estudos</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Engenharia Química e Biológica</t>
+          <t>Engenharia Eletrónica e Telecomunicações e de Computadores</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Nelson Nunes</t>
+          <t>Propinas</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docentes/nelson-guerreiro-cortez-nunes</t>
+          <t>https://www.isel.pt/comunidade/estudantes/informacoes-academicas/propinas</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Engenharia Química e Biológica</t>
+          <t>Engenharia Eletrónica e Telecomunicações e de Computadores</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Sérgio Costa</t>
+          <t>Vitor Costa</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docentes/sergio-jorge-pereira-da-costa</t>
+          <t>https://www.isel.pt/docentes/vitor-manuel-da-silva-costa</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Licenciaturas Comum</t>
+          <t>Engenharia Física Aplicada</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -1422,272 +1422,1853 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Licenciaturas Comum</t>
+          <t>Engenharia Física Aplicada</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Horários</t>
+          <t>Apresentação</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/comunidade/estudantes/informacoes-academicas/horarios</t>
+          <t>https://www.isel.pt/curso/licenciatura/licenciatura-em-engenharia-fisica-aplicada</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Licenciaturas Comum</t>
+          <t>Engenharia Física Aplicada</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>ISEL Student Wins First Prize at the H2O &amp; Sustainability Innovation Hub</t>
+          <t>Congresso do 30.º Aniversário da PROFORUM</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/en/news/isel-student-wins-first-prize-h2o-sustainability-innovation-hub</t>
+          <t>https://www.isel.pt/eventos/congresso-do-30o-aniversario-da-proforum</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Licenciaturas Comum</t>
+          <t>Engenharia Física Aplicada</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Lucía Suárez</t>
+          <t>Descarregar</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docentes/lucia-fernandez-suarez</t>
+          <t>https://isel.pt/sites/default/files/001_imagens_isel/pdf/flyers_2025_04/FolhetoISEL-LEFA.pdf</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Licenciaturas Comum</t>
+          <t>Engenharia Física Aplicada</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Mapa de testes e exames</t>
+          <t>Fundação Santander e ISEL atribuem Incentivo à Investigação Exploratória</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/comunidade/estudantes/informacoes-academicas/testes_e_exames</t>
+          <t>https://www.isel.pt/noticias/fundacao-santander-e-isel-atribuem-incentivo-investigacao-exploratoria</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Licenciaturas Comum</t>
+          <t>Engenharia Física Aplicada</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Modalidades de ingresso</t>
+          <t>Horários</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/ensino/candidatos/modalidades-de-ingresso</t>
+          <t>https://www.isel.pt/comunidade/estudantes/informacoes-academicas/horarios</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Licenciaturas Comum</t>
+          <t>Engenharia Física Aplicada</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Propinas</t>
+          <t>Lucía Suárez</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/comunidade/estudantes/informacoes-academicas/propinas</t>
+          <t>https://www.isel.pt/docentes/lucia-fernandez-suarez</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Licenciaturas Comum</t>
+          <t>Engenharia Física Aplicada</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Seminário de Física - Aplicações ópticas de cristais líquidos</t>
+          <t>Mapa de testes e exames</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/eventos/seminario-de-fisica-aplicacoes-opticas-de-cristais-liquidos-1</t>
+          <t>https://www.isel.pt/comunidade/estudantes/informacoes-academicas/testes_e_exames</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Matemática Aplicada à Tecnologia e à Empresa</t>
+          <t>Engenharia Física Aplicada</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Carlos Geraldes</t>
+          <t>Modalidades de ingresso</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docentes/carlos-jose-bras-geraldes</t>
+          <t>https://www.isel.pt/ensino/candidatos/modalidades-de-ingresso</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Matemática Aplicada à Tecnologia e à Empresa</t>
+          <t>Engenharia Física Aplicada</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Cátia Dias</t>
+          <t>Pedro Ferreira</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docentes/catia-sofia-peniche-lente-dinis-dias</t>
+          <t>https://www.isel.pt/docentes/pedro-miguel-martins-ferreira</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Matemática Aplicada à Tecnologia e à Empresa</t>
+          <t>Engenharia Física Aplicada</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Descarregar</t>
+          <t>Pedro Patrício</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>https://isel.pt/sites/default/files/001_imagens_isel/pdf/flyers_2025_04/FolhetoISEL-LMATE.pdf</t>
+          <t>https://www.isel.pt/docentes/pedro-manuel-alves-patricio-da-silva</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Matemática Aplicada à Tecnologia e à Empresa</t>
+          <t>Engenharia Física Aplicada</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Sandra Aleixo</t>
+          <t>Plano de Estudos</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docentes/sandra-maria-da-silva-figueiredo-aleixo</t>
+          <t>https://www.isel.pt/curso/38165/plano-de-estudos</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Tecnologias e Gestão Municipal</t>
+          <t>Engenharia Física Aplicada</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Descarregar</t>
+          <t>Propinas</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>https://isel.pt/sites/default/files/001_imagens_isel/pdf/flyers_2025_04/FolhetoISEL-LTGM.pdf</t>
+          <t>https://www.isel.pt/comunidade/estudantes/informacoes-academicas/propinas</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Tecnologias e Gestão Municipal</t>
+          <t>Engenharia Física Aplicada</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Luísa Teles Fortes</t>
+          <t>Vitor Oliveira</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docentes/luisa-maria-conceicao-ferreira-cardoso-teles-fortes</t>
+          <t>https://www.isel.pt/docentes/vitor-manuel-barbas-de-oliveira</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Tecnologias e Gestão Municipal</t>
+          <t>Engenharia Informática e Multimédia</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Maria Teresa Santos</t>
+          <t>António Teófilo</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docentes/maria-teresa-loureiro-dos-santos</t>
+          <t>https://www.isel.pt/docentes/antonio-gelasio-frazao-isidro-teofilo</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Tecnologias e Gestão Municipal</t>
+          <t>Engenharia Informática e Multimédia</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Paula Lamego</t>
+          <t>Apresentação</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>https://www.isel.pt/docentes/paula-raquel-pires-da-cunha-lamego</t>
+          <t>https://www.isel.pt/curso/licenciatura/licenciatura-em-engenharia-informatica-e-multimedia</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
+          <t>Engenharia Informática e Multimédia</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>Congresso do 30.º Aniversário da PROFORUM</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>https://www.isel.pt/eventos/congresso-do-30o-aniversario-da-proforum</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>Engenharia Informática e Multimédia</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>Descarregar</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>https://isel.pt/sites/default/files/001_imagens_isel/pdf/flyers_2025_04/FolhetoISEL-LEIM.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>Engenharia Informática e Multimédia</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>Filipa Almeida</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>https://www.isel.pt/docentes/filipa-soares-de-almeida</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>Engenharia Informática e Multimédia</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>Fundação Santander e ISEL atribuem Incentivo à Investigação Exploratória</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>https://www.isel.pt/noticias/fundacao-santander-e-isel-atribuem-incentivo-investigacao-exploratoria</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>Engenharia Informática e Multimédia</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>Gonçalo Valadão Matias</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>https://www.isel.pt/docentes/goncalo-ramiro-valadao-matias</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>Engenharia Informática e Multimédia</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>Horários</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>https://www.isel.pt/comunidade/estudantes/informacoes-academicas/horarios</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>Engenharia Informática e Multimédia</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>Manfred Niehus</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>https://www.isel.pt/docentes/manfred-niehus</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>Engenharia Informática e Multimédia</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>Mapa de testes e exames</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>https://www.isel.pt/comunidade/estudantes/informacoes-academicas/testes_e_exames</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>Engenharia Informática e Multimédia</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>Modalidades de ingresso</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>https://www.isel.pt/ensino/candidatos/modalidades-de-ingresso</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>Engenharia Informática e Multimédia</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>Plano de Estudos</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>https://www.isel.pt/curso/10517/plano-de-estudos</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>Engenharia Informática e Multimédia</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>Propinas</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>https://www.isel.pt/comunidade/estudantes/informacoes-academicas/propinas</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>Engenharia Informática e Multimédia</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>Rui Jesus</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>https://www.isel.pt/docentes/rui-manuel-feliciano-de-jesus</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>Engenharia Informática e de Computadores</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>Apresentação</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>https://www.isel.pt/curso/licenciatura/licenciatura-em-engenharia-informatica-e-de-computadores</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>Engenharia Informática e de Computadores</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>Artur Ferreira</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>https://www.isel.pt/docentes/artur-jorge-ferreira</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>Engenharia Informática e de Computadores</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>Congresso do 30.º Aniversário da PROFORUM</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>https://www.isel.pt/eventos/congresso-do-30o-aniversario-da-proforum</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>Engenharia Informática e de Computadores</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>Cátia Vaz</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>https://www.isel.pt/docentes/catia-raquel-jesus-vaz</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>Engenharia Informática e de Computadores</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>Descarregar</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>https://isel.pt/sites/default/files/001_imagens_isel/pdf/flyers_2025_04/FolhetoISEL-LEIC.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>Engenharia Informática e de Computadores</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>Fundação Santander e ISEL atribuem Incentivo à Investigação Exploratória</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>https://www.isel.pt/noticias/fundacao-santander-e-isel-atribuem-incentivo-investigacao-exploratoria</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>Engenharia Informática e de Computadores</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>Horários</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>https://www.isel.pt/comunidade/estudantes/informacoes-academicas/horarios</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>Engenharia Informática e de Computadores</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>Mapa de testes e exames</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>https://www.isel.pt/comunidade/estudantes/informacoes-academicas/testes_e_exames</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>Engenharia Informática e de Computadores</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>Modalidades de ingresso</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>https://www.isel.pt/ensino/candidatos/modalidades-de-ingresso</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>Engenharia Informática e de Computadores</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>Nuno Leite</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>https://www.isel.pt/docentes/nuno-miguel-da-costa-de-sousa-leite</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>Engenharia Informática e de Computadores</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>Pedro Miguens Matutino</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>https://www.isel.pt/docentes/pedro-miguel-florindo-miguens-matutino</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>Engenharia Informática e de Computadores</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>Plano de Estudos</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>https://www.isel.pt/curso/10514/plano-de-estudos</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>Engenharia Informática e de Computadores</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>Propinas</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>https://www.isel.pt/comunidade/estudantes/informacoes-academicas/propinas</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>Engenharia Informática e de Computadores</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>Testemunhos</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>https://www.isel.pt/leic/testemunhos</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>Engenharia Informática, Redes e Telecomunicações</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>Apresentação</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>https://www.isel.pt/curso/licenciatura/licenciatura-em-engenharia-informatica-redes-e-telecomunicacoes</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>Engenharia Informática, Redes e Telecomunicações</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>Congresso do 30.º Aniversário da PROFORUM</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>https://www.isel.pt/eventos/congresso-do-30o-aniversario-da-proforum</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>Engenharia Informática, Redes e Telecomunicações</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>Descarregar</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>https://isel.pt/sites/default/files/001_imagens_isel/pdf/flyers_2025_04/FolhetoISEL-LEIRT.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>Engenharia Informática, Redes e Telecomunicações</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>Filipe Freitas</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>https://www.isel.pt/docentes/filipe-bastos-de-freitas</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>Engenharia Informática, Redes e Telecomunicações</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>Fundação Santander e ISEL atribuem Incentivo à Investigação Exploratória</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>https://www.isel.pt/noticias/fundacao-santander-e-isel-atribuem-incentivo-investigacao-exploratoria</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>Engenharia Informática, Redes e Telecomunicações</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>Horários</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>https://www.isel.pt/comunidade/estudantes/informacoes-academicas/horarios</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>Engenharia Informática, Redes e Telecomunicações</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>Isabel Matos</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>https://www.isel.pt/docentes/isabel-maria-teixeira-de-matos</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>Engenharia Informática, Redes e Telecomunicações</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>João Trindade</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>https://www.isel.pt/docentes/joao-humberto-holbeche-trindade</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>Engenharia Informática, Redes e Telecomunicações</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>Luis Mata</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>https://www.isel.pt/docente/luis-miguel-maia-bravo-da-mata</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>Engenharia Informática, Redes e Telecomunicações</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>Mapa de testes e exames</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>https://www.isel.pt/comunidade/estudantes/informacoes-academicas/testes_e_exames</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>Engenharia Informática, Redes e Telecomunicações</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>Modalidades de ingresso</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>https://www.isel.pt/ensino/candidatos/modalidades-de-ingresso</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>Engenharia Informática, Redes e Telecomunicações</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>Pedro Vieira</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>https://www.isel.pt/docentes/pedro-manuel-de-almeida-carvalho-vieira</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>Engenharia Informática, Redes e Telecomunicações</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>Plano de Estudos</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>https://www.isel.pt/curso/10564/plano-de-estudos</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>Engenharia Informática, Redes e Telecomunicações</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>Propinas</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>https://www.isel.pt/comunidade/estudantes/informacoes-academicas/propinas</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>Engenharia Mecânica</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>Apresentação</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>https://www.isel.pt/curso/licenciatura/licenciatura-em-engenharia-mecanica</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>Engenharia Mecânica</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>Cláudia Casaca</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>https://www.isel.pt/docentes/claudia-sofia-seneca-da-luz-casaca</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>Engenharia Mecânica</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>Congresso do 30.º Aniversário da PROFORUM</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>https://www.isel.pt/eventos/congresso-do-30o-aniversario-da-proforum</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>Engenharia Mecânica</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>Descarregar</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>https://isel.pt/sites/default/files/001_imagens_isel/pdf/flyers_2025_04/FolhetoISEL-LEM.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>Engenharia Mecânica</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>Fernando Carreira</t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>https://www.isel.pt/docentes/fernando-paulo-neves-da-fonseca-carreira</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>Engenharia Mecânica</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>Fundação Santander e ISEL atribuem Incentivo à Investigação Exploratória</t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>https://www.isel.pt/noticias/fundacao-santander-e-isel-atribuem-incentivo-investigacao-exploratoria</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>Engenharia Mecânica</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>Horários</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>https://www.isel.pt/comunidade/estudantes/informacoes-academicas/horarios</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>Engenharia Mecânica</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>José Sobral</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>https://www.isel.pt/docentes/jose-augusto-da-silva-sobral</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>Engenharia Mecânica</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>Mapa de testes e exames</t>
+        </is>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>https://www.isel.pt/comunidade/estudantes/informacoes-academicas/testes_e_exames</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>Engenharia Mecânica</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>Modalidades de ingresso</t>
+        </is>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>https://www.isel.pt/ensino/candidatos/modalidades-de-ingresso</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>Engenharia Mecânica</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>Plano de Estudos</t>
+        </is>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>https://www.isel.pt/curso/10520/plano-de-estudos</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>Engenharia Mecânica</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>Propinas</t>
+        </is>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>https://www.isel.pt/comunidade/estudantes/informacoes-academicas/propinas</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>Engenharia Mecânica</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>Ricardo Portal</t>
+        </is>
+      </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>https://www.isel.pt/docentes/ricardo-jose-fontes-portal</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>Engenharia Mecânica</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>Teresa Moura e Silva</t>
+        </is>
+      </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>https://www.isel.pt/docentes/maria-teresa-oliveira-moura-e-silva</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>Engenharia Química e Biológica</t>
+        </is>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>Alexandra Costa</t>
+        </is>
+      </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>https://www.isel.pt/docentes/alexandra-isabel-martins-paulo-costa</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>Engenharia Química e Biológica</t>
+        </is>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>Ana Figueiredo</t>
+        </is>
+      </c>
+      <c r="C129" t="inlineStr">
+        <is>
+          <t>https://www.isel.pt/docentes/ana-sofia-de-oliveira-figueiredo</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>Engenharia Química e Biológica</t>
+        </is>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>Apresentação</t>
+        </is>
+      </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>https://www.isel.pt/curso/licenciatura/licenciatura-em-engenharia-quimica-e-biologica</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>Engenharia Química e Biológica</t>
+        </is>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>Congresso do 30.º Aniversário da PROFORUM</t>
+        </is>
+      </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>https://www.isel.pt/eventos/congresso-do-30o-aniversario-da-proforum</t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>Engenharia Química e Biológica</t>
+        </is>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>Descarregar</t>
+        </is>
+      </c>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t>https://isel.pt/sites/default/files/001_imagens_isel/pdf/flyers_2025_04/FolhetoISEL-LEQB.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>Engenharia Química e Biológica</t>
+        </is>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>Fundação Santander e ISEL atribuem Incentivo à Investigação Exploratória</t>
+        </is>
+      </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t>https://www.isel.pt/noticias/fundacao-santander-e-isel-atribuem-incentivo-investigacao-exploratoria</t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>Engenharia Química e Biológica</t>
+        </is>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>Horários</t>
+        </is>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>https://www.isel.pt/comunidade/estudantes/informacoes-academicas/horarios</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>Engenharia Química e Biológica</t>
+        </is>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>Magda Semedo</t>
+        </is>
+      </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>https://www.isel.pt/docentes/magda-sofia-soares-de-carvalho-cardoso-nobre-semedo</t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>Engenharia Química e Biológica</t>
+        </is>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>Mapa de testes e exames</t>
+        </is>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>https://www.isel.pt/comunidade/estudantes/informacoes-academicas/testes_e_exames</t>
+        </is>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>Engenharia Química e Biológica</t>
+        </is>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>Modalidades de ingresso</t>
+        </is>
+      </c>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t>https://www.isel.pt/ensino/candidatos/modalidades-de-ingresso</t>
+        </is>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>Engenharia Química e Biológica</t>
+        </is>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>Nelson Nunes</t>
+        </is>
+      </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>https://www.isel.pt/docentes/nelson-guerreiro-cortez-nunes</t>
+        </is>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>Engenharia Química e Biológica</t>
+        </is>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>Plano de Estudos</t>
+        </is>
+      </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t>https://www.isel.pt/curso/10521/plano-de-estudos</t>
+        </is>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>Engenharia Química e Biológica</t>
+        </is>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>Propinas</t>
+        </is>
+      </c>
+      <c r="C140" t="inlineStr">
+        <is>
+          <t>https://www.isel.pt/comunidade/estudantes/informacoes-academicas/propinas</t>
+        </is>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>Engenharia Química e Biológica</t>
+        </is>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>Sérgio Costa</t>
+        </is>
+      </c>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>https://www.isel.pt/docentes/sergio-jorge-pereira-da-costa</t>
+        </is>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>Matemática Aplicada à Tecnologia e à Empresa</t>
+        </is>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>Apresentação</t>
+        </is>
+      </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>https://www.isel.pt/curso/licenciatura/licenciatura-em-matematica-aplicada-tecnologia-e-empresa</t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>Matemática Aplicada à Tecnologia e à Empresa</t>
+        </is>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>Carlos Geraldes</t>
+        </is>
+      </c>
+      <c r="C143" t="inlineStr">
+        <is>
+          <t>https://www.isel.pt/docentes/carlos-jose-bras-geraldes</t>
+        </is>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>Matemática Aplicada à Tecnologia e à Empresa</t>
+        </is>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>Congresso do 30.º Aniversário da PROFORUM</t>
+        </is>
+      </c>
+      <c r="C144" t="inlineStr">
+        <is>
+          <t>https://www.isel.pt/eventos/congresso-do-30o-aniversario-da-proforum</t>
+        </is>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>Matemática Aplicada à Tecnologia e à Empresa</t>
+        </is>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>Cátia Dias</t>
+        </is>
+      </c>
+      <c r="C145" t="inlineStr">
+        <is>
+          <t>https://www.isel.pt/docentes/catia-sofia-peniche-lente-dinis-dias</t>
+        </is>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>Matemática Aplicada à Tecnologia e à Empresa</t>
+        </is>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>Descarregar</t>
+        </is>
+      </c>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t>https://isel.pt/sites/default/files/001_imagens_isel/pdf/flyers_2025_04/FolhetoISEL-LMATE.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="inlineStr">
+        <is>
+          <t>Matemática Aplicada à Tecnologia e à Empresa</t>
+        </is>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>Fundação Santander e ISEL atribuem Incentivo à Investigação Exploratória</t>
+        </is>
+      </c>
+      <c r="C147" t="inlineStr">
+        <is>
+          <t>https://www.isel.pt/noticias/fundacao-santander-e-isel-atribuem-incentivo-investigacao-exploratoria</t>
+        </is>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="inlineStr">
+        <is>
+          <t>Matemática Aplicada à Tecnologia e à Empresa</t>
+        </is>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>Horários</t>
+        </is>
+      </c>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t>https://www.isel.pt/comunidade/estudantes/informacoes-academicas/horarios</t>
+        </is>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="inlineStr">
+        <is>
+          <t>Matemática Aplicada à Tecnologia e à Empresa</t>
+        </is>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>Lucía Suárez</t>
+        </is>
+      </c>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t>https://www.isel.pt/docentes/lucia-fernandez-suarez</t>
+        </is>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="inlineStr">
+        <is>
+          <t>Matemática Aplicada à Tecnologia e à Empresa</t>
+        </is>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>Mapa de testes e exames</t>
+        </is>
+      </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>https://www.isel.pt/comunidade/estudantes/informacoes-academicas/testes_e_exames</t>
+        </is>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="inlineStr">
+        <is>
+          <t>Matemática Aplicada à Tecnologia e à Empresa</t>
+        </is>
+      </c>
+      <c r="B151" t="inlineStr">
+        <is>
+          <t>Modalidades de ingresso</t>
+        </is>
+      </c>
+      <c r="C151" t="inlineStr">
+        <is>
+          <t>https://www.isel.pt/ensino/candidatos/modalidades-de-ingresso</t>
+        </is>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="inlineStr">
+        <is>
+          <t>Matemática Aplicada à Tecnologia e à Empresa</t>
+        </is>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>Plano de Estudos</t>
+        </is>
+      </c>
+      <c r="C152" t="inlineStr">
+        <is>
+          <t>https://www.isel.pt/curso/10545/plano-de-estudos</t>
+        </is>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="inlineStr">
+        <is>
+          <t>Matemática Aplicada à Tecnologia e à Empresa</t>
+        </is>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>Propinas</t>
+        </is>
+      </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>https://www.isel.pt/comunidade/estudantes/informacoes-academicas/propinas</t>
+        </is>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="inlineStr">
+        <is>
+          <t>Matemática Aplicada à Tecnologia e à Empresa</t>
+        </is>
+      </c>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t>Sandra Aleixo</t>
+        </is>
+      </c>
+      <c r="C154" t="inlineStr">
+        <is>
+          <t>https://www.isel.pt/docentes/sandra-maria-da-silva-figueiredo-aleixo</t>
+        </is>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="inlineStr">
+        <is>
           <t>Tecnologias e Gestão Municipal</t>
         </is>
       </c>
-      <c r="B74" t="inlineStr">
+      <c r="B155" t="inlineStr">
+        <is>
+          <t>Apresentação</t>
+        </is>
+      </c>
+      <c r="C155" t="inlineStr">
+        <is>
+          <t>https://www.isel.pt/curso/licenciatura/licenciatura-em-tecnologias-e-gestao-municipal</t>
+        </is>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="inlineStr">
+        <is>
+          <t>Tecnologias e Gestão Municipal</t>
+        </is>
+      </c>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t>Congresso do 30.º Aniversário da PROFORUM</t>
+        </is>
+      </c>
+      <c r="C156" t="inlineStr">
+        <is>
+          <t>https://www.isel.pt/eventos/congresso-do-30o-aniversario-da-proforum</t>
+        </is>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="inlineStr">
+        <is>
+          <t>Tecnologias e Gestão Municipal</t>
+        </is>
+      </c>
+      <c r="B157" t="inlineStr">
+        <is>
+          <t>Descarregar</t>
+        </is>
+      </c>
+      <c r="C157" t="inlineStr">
+        <is>
+          <t>https://isel.pt/sites/default/files/001_imagens_isel/pdf/flyers_2025_04/FolhetoISEL-LTGM.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr">
+        <is>
+          <t>Tecnologias e Gestão Municipal</t>
+        </is>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>Fundação Santander e ISEL atribuem Incentivo à Investigação Exploratória</t>
+        </is>
+      </c>
+      <c r="C158" t="inlineStr">
+        <is>
+          <t>https://www.isel.pt/noticias/fundacao-santander-e-isel-atribuem-incentivo-investigacao-exploratoria</t>
+        </is>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="inlineStr">
+        <is>
+          <t>Tecnologias e Gestão Municipal</t>
+        </is>
+      </c>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t>Horários</t>
+        </is>
+      </c>
+      <c r="C159" t="inlineStr">
+        <is>
+          <t>https://www.isel.pt/comunidade/estudantes/informacoes-academicas/horarios</t>
+        </is>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="inlineStr">
+        <is>
+          <t>Tecnologias e Gestão Municipal</t>
+        </is>
+      </c>
+      <c r="B160" t="inlineStr">
+        <is>
+          <t>Luísa Teles Fortes</t>
+        </is>
+      </c>
+      <c r="C160" t="inlineStr">
+        <is>
+          <t>https://www.isel.pt/docentes/luisa-maria-conceicao-ferreira-cardoso-teles-fortes</t>
+        </is>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="inlineStr">
+        <is>
+          <t>Tecnologias e Gestão Municipal</t>
+        </is>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>Mapa de testes e exames</t>
+        </is>
+      </c>
+      <c r="C161" t="inlineStr">
+        <is>
+          <t>https://www.isel.pt/comunidade/estudantes/informacoes-academicas/testes_e_exames</t>
+        </is>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="inlineStr">
+        <is>
+          <t>Tecnologias e Gestão Municipal</t>
+        </is>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>Maria Teresa Santos</t>
+        </is>
+      </c>
+      <c r="C162" t="inlineStr">
+        <is>
+          <t>https://www.isel.pt/docentes/maria-teresa-loureiro-dos-santos</t>
+        </is>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="inlineStr">
+        <is>
+          <t>Tecnologias e Gestão Municipal</t>
+        </is>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>Modalidades de ingresso</t>
+        </is>
+      </c>
+      <c r="C163" t="inlineStr">
+        <is>
+          <t>https://www.isel.pt/ensino/candidatos/modalidades-de-ingresso</t>
+        </is>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="inlineStr">
+        <is>
+          <t>Tecnologias e Gestão Municipal</t>
+        </is>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>Paula Lamego</t>
+        </is>
+      </c>
+      <c r="C164" t="inlineStr">
+        <is>
+          <t>https://www.isel.pt/docentes/paula-raquel-pires-da-cunha-lamego</t>
+        </is>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="inlineStr">
+        <is>
+          <t>Tecnologias e Gestão Municipal</t>
+        </is>
+      </c>
+      <c r="B165" t="inlineStr">
         <is>
           <t>Paulo Matos Martins</t>
         </is>
       </c>
-      <c r="C74" t="inlineStr">
+      <c r="C165" t="inlineStr">
         <is>
           <t>https://www.isel.pt/docentes/paulo-jose-de-matos-martins</t>
+        </is>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="inlineStr">
+        <is>
+          <t>Tecnologias e Gestão Municipal</t>
+        </is>
+      </c>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t>Plano de Estudos</t>
+        </is>
+      </c>
+      <c r="C166" t="inlineStr">
+        <is>
+          <t>https://www.isel.pt/curso/10537/plano-de-estudos</t>
+        </is>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="inlineStr">
+        <is>
+          <t>Tecnologias e Gestão Municipal</t>
+        </is>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>Propinas</t>
+        </is>
+      </c>
+      <c r="C167" t="inlineStr">
+        <is>
+          <t>https://www.isel.pt/comunidade/estudantes/informacoes-academicas/propinas</t>
         </is>
       </c>
     </row>

</xml_diff>